<commit_message>
Add SIN function description
</commit_message>
<xml_diff>
--- a/xlsx/tests/docs/SIN.xlsx
+++ b/xlsx/tests/docs/SIN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\Function descriptions\SIN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steve\Documents\IronCalc work\IronCalc-clone\IronCalc-SF\xlsx\tests\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9465601E-A51F-4CAB-B1AA-4D64561BBBE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5890AD01-93E2-4CBA-8DA0-72F5DE100D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{485CA009-6F4A-460D-891C-D7B8869F48AE}"/>
+    <workbookView xWindow="0" yWindow="7200" windowWidth="28800" windowHeight="8280" xr2:uid="{485CA009-6F4A-460D-891C-D7B8869F48AE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Number</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>SIN</t>
+  </si>
+  <si>
+    <t>Formula  Text</t>
+  </si>
+  <si>
+    <t>angle</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Formula Text</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Example of error propagation.</t>
+  </si>
+  <si>
+    <t>Unable to convert angle argument to a number.</t>
+  </si>
+  <si>
+    <t>Input causes a #DIV/0! error.</t>
   </si>
 </sst>
 </file>
@@ -433,10 +454,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{698A441E-9203-46F3-91E3-D681B30E39C3}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,9 +468,12 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="3"/>
@@ -463,6 +487,10 @@
         <f>SIN(A2)</f>
         <v>-1</v>
       </c>
+      <c r="D2" t="str">
+        <f ca="1">_xlfn.FORMULATEXT($B2)</f>
+        <v>=SIN(A2)</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -472,14 +500,22 @@
         <f>SIN(A3)</f>
         <v>-0.47942553860420301</v>
       </c>
+      <c r="D3" t="str">
+        <f t="shared" ref="D3:D7" ca="1" si="0">_xlfn.FORMULATEXT($B3)</f>
+        <v>=SIN(A3)</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B6" si="0">SIN(A4)</f>
+        <f t="shared" ref="B4:B6" si="1">SIN(A4)</f>
         <v>0</v>
+      </c>
+      <c r="D4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SIN(A4)</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -487,8 +523,12 @@
         <v>0.5</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5" si="1">SIN(A5)</f>
+        <f t="shared" ref="B5" si="2">SIN(A5)</f>
         <v>0.47942553860420301</v>
+      </c>
+      <c r="D5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SIN(A5)</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -497,14 +537,73 @@
         <v>1.5707963267948966</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
+      </c>
+      <c r="D6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SIN(A6)</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B7">
         <f>SIN(10*PI()/180)</f>
         <v>0.17364817766693033</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>=SIN(10*PI()/180)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="e">
+        <f>SIN(SQRT(-1))</f>
+        <v>#NUM!</v>
+      </c>
+      <c r="B10" t="str">
+        <f ca="1">_xlfn.FORMULATEXT($A10)</f>
+        <v>=SIN(SQRT(-1))</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="e">
+        <f>SIN("str")</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B11" t="str">
+        <f ca="1">_xlfn.FORMULATEXT($A11)</f>
+        <v>=SIN("str")</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="e">
+        <f>SIN(10/0)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="B12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT($A12)</f>
+        <v>=SIN(10/0)</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>